<commit_message>
Added to DnD and Others
</commit_message>
<xml_diff>
--- a/Dungeons And Dragons stuff/Characters/stats by race.xlsx
+++ b/Dungeons And Dragons stuff/Characters/stats by race.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\awtor\Antonius-Personal\Dungeons And Dragons stuff\Characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77469D12-494B-401C-8250-54740FE42250}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A607AEB7-5EEF-421B-8013-A3D4B6E0EDB6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="960" windowWidth="26445" windowHeight="14790" xr2:uid="{C5BA1E9E-BE21-422B-B8FC-6DCE84E48FCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C5BA1E9E-BE21-422B-B8FC-6DCE84E48FCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,6 +566,9 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -582,6 +585,9 @@
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -609,6 +615,9 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
       <c r="C4">
         <v>1</v>
       </c>
@@ -632,6 +641,9 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
       <c r="C5">
         <v>1</v>
       </c>
@@ -652,6 +664,9 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
       <c r="C6">
         <v>1</v>
       </c>
@@ -666,6 +681,9 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
       <c r="C7">
         <v>1</v>
       </c>
@@ -704,59 +722,59 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" ref="C10:C15" si="0">B2+C2</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ref="D10:D15" si="1">B2+D2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ref="E10:E15" si="2">B2+E2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F10" s="3">
         <f>B2+F2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G10" s="3">
         <f>B2+G2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H10" s="3">
         <f>B2+H2</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I10" s="3">
         <f>B2+I2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J10" s="3">
         <f>B2+J2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K10" s="3">
         <f>B2+K2</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="L10" s="3">
         <f>B2+L2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M10" s="3">
         <f>B2+M2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N10" s="3">
         <f>B2+N2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O10" s="3">
         <f>B2+O2</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="P10" s="3">
         <f>B2+P2</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -765,59 +783,59 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <f t="shared" ref="F11:F15" si="3">B3+F3</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G15" si="4">B3+G3</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H15" si="5">B3+H3</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I11">
         <f t="shared" ref="I11:I15" si="6">B3+I3</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J15" si="7">B3+J3</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K15" si="8">B3+K3</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L11">
         <f t="shared" ref="L11:L15" si="9">B3+L3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M11">
         <f t="shared" ref="M11:M15" si="10">B3+M3</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N15" si="11">B3+N3</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O11">
         <f t="shared" ref="O11:O15" si="12">B3+O3</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P15" si="13">B3+P3</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -826,59 +844,59 @@
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E12" s="4">
         <f>B4+E4</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K12" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="M12" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="O12" s="4">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="P12" s="4">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -887,59 +905,59 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G13">
         <f>B5+G5</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J13">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K13">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L13">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="M13">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="N13">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O13">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="P13">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -948,59 +966,59 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I14" s="5">
         <f>B6+I6</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O14" s="5">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P14" s="5">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1009,59 +1027,59 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H15">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K15">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="L15">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M15">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N15">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="O15">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="P15">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1131,59 +1149,59 @@
       </c>
       <c r="C17">
         <f>SUM(C10:C16)</f>
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="D17">
         <f t="shared" ref="D17:P17" si="15">SUM(D10:D16)</f>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="E17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="F17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="G17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="H17">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="I17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="J17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="K17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="L17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="M17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="N17">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="O17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="P17">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>